<commit_message>
Last version with tests
</commit_message>
<xml_diff>
--- a/src/main/resources/requestFile.xlsx
+++ b/src/main/resources/requestFile.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Java\UTHttpURLConnection\src\main\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="90" windowWidth="19155" windowHeight="8520"/>
+    <workbookView xWindow="21630" yWindow="90" windowWidth="19155" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="request" sheetId="1" r:id="rId1"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>requestType</t>
   </si>
@@ -102,17 +107,62 @@
     <t>4111111111111111</t>
   </si>
   <si>
-    <t>30301</t>
-  </si>
-  <si>
     <t>12500</t>
+  </si>
+  <si>
+    <t>accountData</t>
+  </si>
+  <si>
+    <t>(~2001)021301000F3D0000%*4111********1111^SMITH/JOHN^*****************************?*8D40AD26E14C98F73B0210CD5F18A62ACF2B655EABC19BC10DAEEB870B42D6EADC20CE84E3677286B56D6F1CB7C4276C6BF10A91DB9E5947CA68AFD5884C2737312165237673628FB321C9B5F5094594C71F123CE8980E3482F3CB89629949003A0002E000E759D903</t>
+  </si>
+  <si>
+    <t>7500</t>
+  </si>
+  <si>
+    <t>13500</t>
+  </si>
+  <si>
+    <t>11111</t>
+  </si>
+  <si>
+    <t>22222</t>
+  </si>
+  <si>
+    <t>33333</t>
+  </si>
+  <si>
+    <t>44444</t>
+  </si>
+  <si>
+    <t>111</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>333</t>
+  </si>
+  <si>
+    <t>444</t>
+  </si>
+  <si>
+    <t>csc</t>
+  </si>
+  <si>
+    <t>splits</t>
+  </si>
+  <si>
+    <t>13 Main St</t>
+  </si>
+  <si>
+    <t>14 Main St</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -121,12 +171,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
       <b/>
       <sz val="9"/>
-      <color rgb="FF008000"/>
       <name val="Courier New"/>
       <family val="3"/>
       <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -137,7 +211,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -145,16 +219,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="mediumDashed">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="mediumDashed">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="mediumDashed">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="mediumDashed">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -164,6 +259,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -212,7 +310,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,7 +345,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -456,170 +554,310 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O3"/>
+  <dimension ref="A1:R9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="R2" sqref="R2:R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.28515625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="17.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="7.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="6.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.7109375" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:18" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="3" t="s">
         <v>13</v>
       </c>
+      <c r="Q1" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="R1" s="5" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:18" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="1" t="s">
+      <c r="G2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="R2" s="5"/>
+    </row>
+    <row r="3" spans="1:18" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P3" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="R3" s="5"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="4" spans="1:18" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
+      <c r="C4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="F4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K3" s="1" t="s">
+      <c r="K4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M4" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="N4" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P4" s="3" t="s">
         <v>23</v>
       </c>
+      <c r="Q4" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R4" s="5"/>
+    </row>
+    <row r="5" spans="1:18" s="6" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="M5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="O5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="R5" s="5"/>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q6" s="2"/>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q7" s="2"/>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q8" s="2"/>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="Q9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>